<commit_message>
Deploying to gh-pages from  @ 19a801383f1c9bd9beab453522889d05a2b50951 🚀
</commit_message>
<xml_diff>
--- a/2021-01-04.xlsx
+++ b/2021-01-04.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projekte\Abt3_IQM-COVID19\Fachlich\Auswertungen\2021-01-03\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Projekte\Abt3_IQM-COVID19\Fachlich\Auswertungen\2021-01-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FBA535F-0D4D-4F07-954D-56045E610368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78EB11F1-4D0E-4889-8A4C-DCF260BF9705}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterung" sheetId="9" r:id="rId1"/>
-    <sheet name="02.01.21" sheetId="6" r:id="rId2"/>
+    <sheet name="03.01.21" sheetId="6" r:id="rId2"/>
+    <sheet name="Impfungen_proTag" sheetId="10" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="Bundesländer001" localSheetId="1">'02.01.21'!$A$1:$G$17</definedName>
+    <definedName name="Bundesländer001" localSheetId="1">'03.01.21'!$A$1:$I$17</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <t>Bayern</t>
   </si>
@@ -100,9 +101,6 @@
     <t>Impfungen kumulativ</t>
   </si>
   <si>
-    <t>Gemeldete Impfungen bundesweit und nach Bundesland sowie nach STIKO-Indikation</t>
-  </si>
-  <si>
     <t xml:space="preserve">Die kumulative Zahl der Impfungen umfasst die mit jeweiligem Datenstand gemeldeten Impfungen an das RKI. </t>
   </si>
   <si>
@@ -112,7 +110,13 @@
     <t>Datenstand: 28.12.2020, 08:00 Uhr</t>
   </si>
   <si>
-    <t>08:00 Uhr</t>
+    <t xml:space="preserve">Die Impfquote ist der Anteil aller bisher Geimpften in der Gesamtbevölkerung. </t>
+  </si>
+  <si>
+    <t>Für die Berechnung der Impfquote wurde der Bevölkerungsstand vom 31.12.2019 zugrunde gelegt (Quelle: Statistisches Bundesamt, https://www.destatis.de/DE/Themen/Gesellschaft-Umwelt/Bevoelkerung/Bevoelkerungsstand/Tabellen/bevoelkerung-nichtdeutsch-laender.html).</t>
+  </si>
+  <si>
+    <t>Anmerkung zu den Indikationen: es können mehrere Indikationen je geimpfter Person vorliegen</t>
   </si>
   <si>
     <t>Indikation nach Alter*</t>
@@ -133,20 +137,39 @@
     <t>* In einigen Bundesländern werden nicht alle der in der Tabelle aufgeführten Indikationen einzeln ausgewiesen.</t>
   </si>
   <si>
-    <t>(Nachmeldungen der mobilen Teams stehen noch aus)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(keine Meldung für den 02.01.; Nachmeldung erfolgt am 04.01.2020) </t>
+    <t>Impfungen pro 1.000 Einwohner</t>
+  </si>
+  <si>
+    <t>(Meldung vom 03.01. steht noch aus)</t>
+  </si>
+  <si>
+    <t>Gesamtzahl Impfungen</t>
+  </si>
+  <si>
+    <t>12:00 Uhr</t>
+  </si>
+  <si>
+    <t>Gemeldete Impfungen bundesweit und nach Bundesland sowie nach STIKO-Indikation (03.01.21)</t>
+  </si>
+  <si>
+    <t>Diese Zahl umfasst die mit jeweiligem Datenstand gemeldeten Impfungen an das RKI.</t>
+  </si>
+  <si>
+    <t>Gemeldete Impfungen bundesweit nach Tag der Impfung (Impfungen_proTag)</t>
+  </si>
+  <si>
+    <t>Datum der Impfung</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0"/>
+    <numFmt numFmtId="165" formatCode="#,##0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -201,8 +224,36 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF1A1A1A"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -227,8 +278,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -288,13 +351,28 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -303,9 +381,6 @@
     <xf numFmtId="3" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -324,9 +399,15 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="3" fontId="1" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -334,6 +415,9 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -344,14 +428,39 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="6" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -375,19 +484,19 @@
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Bundesländer001" fillFormulas="1" connectionId="1" xr16:uid="{3DDBA091-D29F-447B-8304-A418A1635D4F}" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh preserveSortFilterLayout="0" nextId="11">
-    <queryTableFields count="7">
+    <queryTableFields count="8">
       <queryTableField id="1" name="Bundesland"/>
       <queryTableField id="2" name="Fälle kumulativ"/>
       <queryTableField id="3" name="Differenz Vortag"/>
+      <queryTableField id="4" name="Fälle kumulativ/ 100.000 Einw."/>
       <queryTableField id="5" name="Fälle in den letzten 7 Tagen"/>
       <queryTableField id="10" dataBound="0" fillFormulas="1"/>
       <queryTableField id="9" dataBound="0" fillFormulas="1"/>
       <queryTableField id="6" name="7-Tage-Inzidenz"/>
     </queryTableFields>
-    <queryTableDeletedFields count="3">
+    <queryTableDeletedFields count="2">
       <deletedField name="Todesfälle"/>
       <deletedField name="Todesfälle/ 100.000 Einw."/>
-      <deletedField name="Fälle kumulativ/ 100.000 Einw."/>
     </queryTableDeletedFields>
   </queryTableRefresh>
 </queryTable>
@@ -714,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5241AA5B-8CBB-47B1-9317-352256D0A517}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,59 +843,67 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="B3" s="20">
+        <f ca="1">TODAY()</f>
+        <v>44200</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="20"/>
+      <c r="C4" s="21"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B6" s="18">
-        <f ca="1">TODAY()</f>
-        <v>44199</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>26</v>
-      </c>
+      <c r="A5" s="33" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="34" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" s="22" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="32" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -797,437 +914,591 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8185A2DF-1594-45F9-85B9-EB1F8407882D}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L24" sqref="L24:L25"/>
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
-    <col min="7" max="7" width="14.28515625" customWidth="1"/>
+    <col min="4" max="4" width="13" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="8" max="8" width="14.28515625" customWidth="1"/>
+    <col min="9" max="9" width="36" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="D1" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="12" t="s">
+      <c r="G1" s="10" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H1" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="13">
-        <v>24063</v>
-      </c>
-      <c r="C2" s="8">
-        <v>4014</v>
-      </c>
-      <c r="D2" s="7">
-        <v>11041</v>
-      </c>
-      <c r="E2" s="8">
-        <v>7428</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1382</v>
-      </c>
-      <c r="G2" s="21">
-        <v>4200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>27454</v>
+      </c>
+      <c r="C2" s="7">
+        <v>3390</v>
+      </c>
+      <c r="D2" s="23">
+        <v>2.4732455442572578</v>
+      </c>
+      <c r="E2" s="6">
+        <v>12584</v>
+      </c>
+      <c r="F2" s="7">
+        <v>8739</v>
+      </c>
+      <c r="G2" s="7">
+        <v>1469</v>
+      </c>
+      <c r="H2" s="14">
+        <v>4932</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="15">
-        <v>57833</v>
-      </c>
-      <c r="C3" s="16">
-        <v>11742</v>
-      </c>
-      <c r="D3" s="17">
-        <v>12855</v>
-      </c>
-      <c r="E3" s="16">
-        <v>25636</v>
-      </c>
-      <c r="F3" s="16">
-        <v>1091</v>
-      </c>
-      <c r="G3" s="22">
-        <v>20428</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B3" s="16">
+        <v>66258</v>
+      </c>
+      <c r="C3" s="17">
+        <v>8425</v>
+      </c>
+      <c r="D3" s="24">
+        <v>5.0483297303405017</v>
+      </c>
+      <c r="E3" s="19">
+        <v>15480</v>
+      </c>
+      <c r="F3" s="17">
+        <v>31755</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1280</v>
+      </c>
+      <c r="H3" s="18">
+        <v>23823</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="13">
-        <v>14616</v>
-      </c>
-      <c r="C4" s="8">
-        <v>1443</v>
-      </c>
-      <c r="D4" s="7">
-        <v>9817</v>
-      </c>
-      <c r="E4" s="8">
-        <v>3647</v>
-      </c>
-      <c r="F4" s="8">
+        <v>17758</v>
+      </c>
+      <c r="C4" s="7">
+        <v>935</v>
+      </c>
+      <c r="D4" s="23">
+        <v>4.8393632795393149</v>
+      </c>
+      <c r="E4" s="6">
+        <v>10507</v>
+      </c>
+      <c r="F4" s="7">
+        <v>6132</v>
+      </c>
+      <c r="G4" s="7">
         <v>105</v>
       </c>
-      <c r="G4" s="21">
-        <v>10968</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H4" s="14">
+        <v>11625</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="15">
-        <v>3219</v>
-      </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="17">
+      <c r="B5" s="16">
+        <v>3309</v>
+      </c>
+      <c r="C5" s="17"/>
+      <c r="D5" s="24">
+        <v>1.3121095938646088</v>
+      </c>
+      <c r="E5" s="19">
         <v>204</v>
       </c>
-      <c r="E5" s="16">
-        <v>2995</v>
-      </c>
-      <c r="F5" s="16">
+      <c r="F5" s="17">
+        <v>3085</v>
+      </c>
+      <c r="G5" s="17">
         <v>20</v>
       </c>
-      <c r="G5" s="22">
+      <c r="H5" s="18">
         <v>224</v>
       </c>
-      <c r="H5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="13">
-        <v>1837</v>
-      </c>
-      <c r="C6" s="8">
-        <v>96</v>
-      </c>
-      <c r="D6" s="7">
+        <v>1903</v>
+      </c>
+      <c r="C6" s="7">
+        <v>66</v>
+      </c>
+      <c r="D6" s="23">
+        <v>2.7935913282697351</v>
+      </c>
+      <c r="E6" s="6">
         <v>824</v>
       </c>
-      <c r="E6" s="8">
-        <v>465</v>
-      </c>
-      <c r="F6" s="8">
+      <c r="F6" s="7">
+        <v>506</v>
+      </c>
+      <c r="G6" s="7">
         <v>9</v>
       </c>
-      <c r="G6" s="21">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H6" s="14">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="15">
-        <v>3704</v>
-      </c>
-      <c r="C7" s="16">
-        <v>662</v>
-      </c>
-      <c r="D7" s="17">
-        <v>1439</v>
-      </c>
-      <c r="E7" s="16">
-        <v>2010</v>
-      </c>
-      <c r="F7" s="16"/>
-      <c r="G7" s="22">
-        <v>1696</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="16">
+        <v>4140</v>
+      </c>
+      <c r="C7" s="17">
+        <v>436</v>
+      </c>
+      <c r="D7" s="24">
+        <v>2.2411656659916104</v>
+      </c>
+      <c r="E7" s="19">
+        <v>1616</v>
+      </c>
+      <c r="F7" s="17">
+        <v>2189</v>
+      </c>
+      <c r="G7" s="17">
+        <v>0</v>
+      </c>
+      <c r="H7" s="18">
+        <v>1953</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="B8" s="13">
-        <v>30085</v>
-      </c>
-      <c r="C8" s="8">
-        <v>5294</v>
-      </c>
-      <c r="D8" s="7">
-        <v>8443</v>
-      </c>
-      <c r="E8" s="8">
-        <v>17635</v>
-      </c>
-      <c r="F8" s="8">
-        <v>1096</v>
-      </c>
-      <c r="G8" s="21">
-        <v>11569</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>33405</v>
+      </c>
+      <c r="C8" s="7">
+        <v>3320</v>
+      </c>
+      <c r="D8" s="23">
+        <v>5.3124324118013764</v>
+      </c>
+      <c r="E8" s="6">
+        <v>9387</v>
+      </c>
+      <c r="F8" s="7">
+        <v>19405</v>
+      </c>
+      <c r="G8" s="7">
+        <v>1185</v>
+      </c>
+      <c r="H8" s="14">
+        <v>12955</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="16">
         <v>11494</v>
       </c>
-      <c r="C9" s="16"/>
-      <c r="D9" s="17">
+      <c r="C9" s="17"/>
+      <c r="D9" s="24">
+        <v>7.1473965542758151</v>
+      </c>
+      <c r="E9" s="19">
         <v>178</v>
       </c>
-      <c r="E9" s="16">
+      <c r="F9" s="17">
         <v>6583</v>
       </c>
-      <c r="F9" s="16">
+      <c r="G9" s="17">
         <v>8</v>
       </c>
-      <c r="G9" s="22">
+      <c r="H9" s="18">
         <v>4804</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="13">
-        <v>4962</v>
-      </c>
-      <c r="C10" s="8">
-        <v>1017</v>
-      </c>
-      <c r="D10" s="7">
-        <v>912</v>
-      </c>
-      <c r="E10" s="8">
-        <v>2641</v>
-      </c>
-      <c r="F10" s="8">
-        <v>982</v>
-      </c>
-      <c r="G10" s="21">
-        <v>2918</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>5394</v>
+      </c>
+      <c r="C10" s="7">
+        <v>432</v>
+      </c>
+      <c r="D10" s="23">
+        <v>0.67478915653607241</v>
+      </c>
+      <c r="E10" s="6">
+        <v>992</v>
+      </c>
+      <c r="F10" s="7">
+        <v>2822</v>
+      </c>
+      <c r="G10" s="7">
+        <v>1035</v>
+      </c>
+      <c r="H10" s="14">
+        <v>3178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="15">
-        <v>48691</v>
-      </c>
-      <c r="C11" s="16">
-        <v>13142</v>
-      </c>
-      <c r="D11" s="17"/>
-      <c r="E11" s="16">
-        <v>18806</v>
-      </c>
-      <c r="F11" s="16"/>
-      <c r="G11" s="22">
-        <v>29893</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B11" s="16">
+        <v>53841</v>
+      </c>
+      <c r="C11" s="17">
+        <v>3539</v>
+      </c>
+      <c r="D11" s="24">
+        <v>2.9999630583475851</v>
+      </c>
+      <c r="E11" s="19">
+        <v>0</v>
+      </c>
+      <c r="F11" s="17">
+        <v>21354</v>
+      </c>
+      <c r="G11" s="17">
+        <v>0</v>
+      </c>
+      <c r="H11" s="18">
+        <v>32495</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="13">
         <v>7248</v>
       </c>
-      <c r="C12" s="8">
-        <v>59</v>
-      </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="8">
+      <c r="C12" s="7"/>
+      <c r="D12" s="23">
+        <v>1.7704376483761339</v>
+      </c>
+      <c r="E12" s="6">
+        <v>0</v>
+      </c>
+      <c r="F12" s="7">
         <v>3516</v>
       </c>
-      <c r="F12" s="8"/>
-      <c r="G12" s="21">
+      <c r="G12" s="7">
+        <v>0</v>
+      </c>
+      <c r="H12" s="14">
         <v>3732</v>
       </c>
-      <c r="H12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="16">
         <v>4149</v>
       </c>
-      <c r="C13" s="16">
-        <v>833</v>
-      </c>
-      <c r="D13" s="17">
+      <c r="C13" s="17"/>
+      <c r="D13" s="24">
+        <v>4.2041287401698471</v>
+      </c>
+      <c r="E13" s="19">
         <v>3122</v>
       </c>
-      <c r="E13" s="16">
+      <c r="F13" s="17">
         <v>495</v>
       </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="22">
+      <c r="G13" s="17">
+        <v>0</v>
+      </c>
+      <c r="H13" s="18">
         <v>1580</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B14" s="13">
-        <v>4343</v>
-      </c>
-      <c r="C14" s="8">
-        <v>343</v>
-      </c>
-      <c r="D14" s="7">
-        <v>368</v>
-      </c>
-      <c r="E14" s="8">
-        <v>3535</v>
-      </c>
-      <c r="F14" s="8">
+        <v>4866</v>
+      </c>
+      <c r="C14" s="7">
+        <v>523</v>
+      </c>
+      <c r="D14" s="23">
+        <v>1.194998687367862</v>
+      </c>
+      <c r="E14" s="6">
+        <v>487</v>
+      </c>
+      <c r="F14" s="7">
+        <v>3765</v>
+      </c>
+      <c r="G14" s="7">
         <v>1</v>
       </c>
-      <c r="G14" s="21">
-        <v>807</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H14" s="14">
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B15" s="15">
-        <v>12822</v>
-      </c>
-      <c r="C15" s="16">
-        <v>1051</v>
-      </c>
-      <c r="D15" s="17">
-        <v>4237</v>
-      </c>
-      <c r="E15" s="16">
-        <v>6194</v>
-      </c>
-      <c r="F15" s="16">
-        <v>546</v>
-      </c>
-      <c r="G15" s="22">
-        <v>6410</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="16">
+        <v>13366</v>
+      </c>
+      <c r="C15" s="17">
+        <v>544</v>
+      </c>
+      <c r="D15" s="24">
+        <v>6.0898986778641344</v>
+      </c>
+      <c r="E15" s="19">
+        <v>4391</v>
+      </c>
+      <c r="F15" s="17">
+        <v>6446</v>
+      </c>
+      <c r="G15" s="17">
+        <v>562</v>
+      </c>
+      <c r="H15" s="18">
+        <v>6702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="13">
-        <v>8933</v>
-      </c>
-      <c r="C16" s="8">
-        <v>969</v>
-      </c>
-      <c r="D16" s="7">
-        <v>2525</v>
-      </c>
-      <c r="E16" s="8">
-        <v>5136</v>
-      </c>
-      <c r="F16" s="8">
-        <v>2077</v>
-      </c>
-      <c r="G16" s="21">
-        <v>3987</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>9557</v>
+      </c>
+      <c r="C16" s="7">
+        <v>624</v>
+      </c>
+      <c r="D16" s="23">
+        <v>3.2912352308531005</v>
+      </c>
+      <c r="E16" s="6">
+        <v>2801</v>
+      </c>
+      <c r="F16" s="7">
+        <v>5317</v>
+      </c>
+      <c r="G16" s="7">
+        <v>2325</v>
+      </c>
+      <c r="H16" s="14">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="15">
+      <c r="B17" s="16">
         <v>810</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="17">
+      <c r="C17" s="17"/>
+      <c r="D17" s="24">
+        <v>0.37967955045941226</v>
+      </c>
+      <c r="E17" s="17">
         <v>232</v>
       </c>
-      <c r="E17" s="16">
+      <c r="F17" s="17">
         <v>297</v>
       </c>
-      <c r="F17" s="16"/>
-      <c r="G17" s="22">
+      <c r="G17" s="17">
+        <v>0</v>
+      </c>
+      <c r="H17" s="18">
         <v>413</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="14">
-        <f>SUM(B2:B17)</f>
-        <v>238809</v>
-      </c>
-      <c r="C18" s="14">
-        <f>SUM(C2:C17)</f>
-        <v>40665</v>
-      </c>
-      <c r="D18" s="9">
-        <f t="shared" ref="D18" si="0">SUM(D2:D17)</f>
-        <v>56197</v>
-      </c>
-      <c r="E18" s="10">
-        <f>SUM(E2:E17)</f>
-        <v>107019</v>
-      </c>
-      <c r="F18" s="10">
-        <f>SUM(F2:F17)</f>
-        <v>7317</v>
-      </c>
-      <c r="G18" s="23">
-        <f>SUM(G2:G17)</f>
-        <v>103894</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="15">
+        <v>264952</v>
+      </c>
+      <c r="C18" s="15">
+        <v>22234</v>
+      </c>
+      <c r="D18" s="25">
+        <v>3.1857938929435359</v>
+      </c>
+      <c r="E18" s="8">
+        <v>62805</v>
+      </c>
+      <c r="F18" s="9">
+        <v>122406</v>
+      </c>
+      <c r="G18" s="9">
+        <v>7999</v>
+      </c>
+      <c r="H18" s="26">
+        <v>114317</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="20" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="22" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926B42D2-7956-44E7-BD5B-5AF896796AC0}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="28" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="29">
+        <v>44192</v>
+      </c>
+      <c r="B2" s="30">
+        <v>23224</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="31">
+        <f>A2+1</f>
+        <v>44193</v>
+      </c>
+      <c r="B3" s="30">
+        <v>17974</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="31">
+        <f t="shared" ref="A4:A9" si="0">A3+1</f>
+        <v>44194</v>
+      </c>
+      <c r="B4" s="30">
+        <v>40187</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="31">
+        <f t="shared" si="0"/>
+        <v>44195</v>
+      </c>
+      <c r="B5" s="30">
+        <v>54322</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="31">
+        <f t="shared" si="0"/>
+        <v>44196</v>
+      </c>
+      <c r="B6" s="30">
+        <v>35498</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="31">
+        <f t="shared" si="0"/>
+        <v>44197</v>
+      </c>
+      <c r="B7" s="30">
+        <v>29712</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="31">
+        <f t="shared" si="0"/>
+        <v>44198</v>
+      </c>
+      <c r="B8" s="30">
+        <v>41801</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="31">
+        <f t="shared" si="0"/>
+        <v>44199</v>
+      </c>
+      <c r="B9" s="30">
+        <v>22234</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>